<commit_message>
q2 optimisation, decision tree template
</commit_message>
<xml_diff>
--- a/Assignment 2/optim1.xlsx
+++ b/Assignment 2/optim1.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="480" windowWidth="16180" windowHeight="10300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="480" windowWidth="16180" windowHeight="10300" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
   <si>
     <t>Brazil</t>
   </si>
@@ -61,6 +62,27 @@
   </si>
   <si>
     <t>Asia</t>
+  </si>
+  <si>
+    <t>Brazilian Real</t>
+  </si>
+  <si>
+    <t>Euro</t>
+  </si>
+  <si>
+    <t>Indian Rupee</t>
+  </si>
+  <si>
+    <t>Japanese Yen</t>
+  </si>
+  <si>
+    <t>Mexican Peso</t>
+  </si>
+  <si>
+    <t>US Dollar</t>
+  </si>
+  <si>
+    <t>Changes in Exchange Rates</t>
   </si>
 </sst>
 </file>
@@ -739,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,4 +1091,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>0.93580249999999998</v>
+      </c>
+      <c r="C2">
+        <v>0.95286199999999999</v>
+      </c>
+      <c r="D2">
+        <v>1.0548793999999999</v>
+      </c>
+      <c r="E2">
+        <v>1.1045636999999999</v>
+      </c>
+      <c r="F2">
+        <v>1.0747187</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed typo for Q1 and Q2, added new quantities into excel file sheet1 and 2
</commit_message>
<xml_diff>
--- a/Assignment 2/optim1.xlsx
+++ b/Assignment 2/optim1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aejl/lsca_group/Assignment 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\lsca_group\Assignment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="11000" windowHeight="11780" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="11000" windowHeight="11780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -110,6 +110,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -380,16 +383,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="A1:H13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -435,7 +438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -458,7 +461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -484,7 +487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -507,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -533,7 +536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -556,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -582,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -605,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -631,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -654,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -680,7 +683,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -713,11 +716,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
@@ -725,7 +728,7 @@
     <col min="7" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -747,7 +750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -773,7 +776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -797,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -823,13 +826,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -841,13 +844,13 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>11000000</v>
+        <v>7000000</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -873,7 +876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -897,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -905,10 +908,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="D8" s="1">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="E8" s="1">
         <v>2000000</v>
@@ -923,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -947,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -973,7 +976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
@@ -997,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -1017,13 +1020,13 @@
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>13000000</v>
+        <v>17000000</v>
       </c>
       <c r="H12" s="1">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>8</v>
@@ -1061,12 +1064,12 @@
       <selection activeCell="H13" sqref="A1:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1088,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1138,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1164,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1188,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1238,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1264,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -1288,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
@@ -1338,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1364,7 +1367,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>8</v>
@@ -1398,13 +1401,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1426,7 +1429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1452,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1476,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1502,7 +1505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1526,7 +1529,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1552,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1576,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -1626,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1652,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
@@ -1676,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fixed the typo of US import tarriff 0.4 to 0.04, altered excel sheets to reflect this and the rmd and HTML comments, didn't touch section concerning exchange rates and decision tree.
</commit_message>
<xml_diff>
--- a/Assignment 2/optim1.xlsx
+++ b/Assignment 2/optim1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="11000" windowHeight="11780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="11000" windowHeight="11780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -716,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -1060,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="A1:H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1173,7 +1173,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -1185,10 +1185,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>11000000</v>
+        <v>7000000</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1249,13 +1249,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="1">
+        <v>4000000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
         <v>3000000</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2000000</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2000000</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -1352,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -1361,10 +1361,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>13000000</v>
+        <v>17000000</v>
       </c>
       <c r="H12" s="1">
-        <v>6000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>